<commit_message>
Various fixes to matches
Lots of random missing player info.
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016-orl-ptfc-062616.xlsx
+++ b/source/excel/nwsl-2016-orl-ptfc-062616.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Documents/GitHub/wosostats/source/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25AA86A-BF80-C947-9C39-CF9ED7DB86BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="780" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="5200" yWindow="660" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -20,10 +21,18 @@
     <definedName name="_FilterDatabase_0" localSheetId="0">match!$A$1:$T$1517</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">match!$A$1:$T$1517</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19696" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19698" uniqueCount="265">
   <si>
     <t>event</t>
   </si>
@@ -833,7 +842,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1114,6 +1123,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1380,12 +1392,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1517"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1388" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1394" sqref="Q1394"/>
+      <pane ySplit="1" topLeftCell="A856" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D871" sqref="D871"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51848,8 +51860,12 @@
       <c r="C872" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D872" s="1"/>
-      <c r="E872" s="1"/>
+      <c r="D872" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E872" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="F872" s="16" t="s">
         <v>210</v>
       </c>
@@ -79883,13 +79899,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1517"/>
+  <autoFilter ref="A1:T1517" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>